<commit_message>
new task for sprint 2
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_RED.xlsx
+++ b/doc/task10/scrum_RED.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="155">
   <si>
     <t>ID</t>
   </si>
@@ -509,6 +509,18 @@
   </si>
   <si>
     <t>Navigation for UI</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>State Pattern</t>
+  </si>
+  <si>
+    <t>implementation of the state pattern</t>
+  </si>
+  <si>
+    <t>...</t>
   </si>
 </sst>
 </file>
@@ -689,7 +701,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -751,6 +763,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1520,10 +1535,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,10 +1548,11 @@
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="9" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1562,13 +1578,13 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="28" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="28" t="s">
         <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1597,10 +1613,10 @@
       <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="9">
         <v>2</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="9">
         <v>2</v>
       </c>
       <c r="K2" t="s">
@@ -1629,10 +1645,10 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="9">
         <v>5</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="9">
         <v>2</v>
       </c>
       <c r="K3" t="s">
@@ -1658,10 +1674,10 @@
       <c r="F4" t="s">
         <v>91</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9">
         <v>1</v>
       </c>
       <c r="K4" t="s">
@@ -1687,7 +1703,7 @@
       <c r="F5" t="s">
         <v>91</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="9">
         <v>3</v>
       </c>
       <c r="K5" t="s">
@@ -1713,10 +1729,10 @@
       <c r="F6" t="s">
         <v>96</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="9">
         <v>10</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="9">
         <v>19</v>
       </c>
       <c r="K6" t="s">
@@ -1742,10 +1758,10 @@
       <c r="F7" t="s">
         <v>106</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="9">
         <v>4</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="9">
         <v>5</v>
       </c>
       <c r="K7" t="s">
@@ -1771,10 +1787,10 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="9">
         <v>2</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="9">
         <v>2</v>
       </c>
       <c r="K8" t="s">
@@ -1800,10 +1816,10 @@
       <c r="F9" t="s">
         <v>97</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="9">
         <v>3</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
@@ -1829,10 +1845,10 @@
       <c r="F10" t="s">
         <v>97</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="9">
         <v>2</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="9">
         <v>1</v>
       </c>
       <c r="K10" t="s">
@@ -1858,10 +1874,10 @@
       <c r="F11" t="s">
         <v>97</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="J11">
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="J11" s="9">
         <v>0</v>
       </c>
       <c r="K11" t="s">
@@ -1887,10 +1903,10 @@
       <c r="F12" t="s">
         <v>97</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="J12">
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+      <c r="J12" s="9">
         <v>1</v>
       </c>
       <c r="K12" t="s">
@@ -1916,10 +1932,10 @@
       <c r="F13" t="s">
         <v>97</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="J13">
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="J13" s="9">
         <v>1</v>
       </c>
       <c r="K13" t="s">
@@ -1945,7 +1961,7 @@
       <c r="F14" t="s">
         <v>97</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="9">
         <v>2</v>
       </c>
       <c r="K14" t="s">
@@ -1974,7 +1990,7 @@
       <c r="G16" t="s">
         <v>5</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="9">
         <v>1</v>
       </c>
       <c r="K16" t="s">
@@ -2003,7 +2019,7 @@
       <c r="G17" t="s">
         <v>5</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="9">
         <v>2</v>
       </c>
       <c r="K17" t="s">
@@ -2032,7 +2048,7 @@
       <c r="G18" t="s">
         <v>6</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="9">
         <v>2</v>
       </c>
       <c r="K18" t="s">
@@ -2061,7 +2077,7 @@
       <c r="G19" t="s">
         <v>6</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="9">
         <v>2</v>
       </c>
       <c r="K19" t="s">
@@ -2090,7 +2106,7 @@
       <c r="G20" t="s">
         <v>5</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="9">
         <v>2</v>
       </c>
       <c r="K20" t="s">
@@ -2119,7 +2135,7 @@
       <c r="G21" t="s">
         <v>5</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="9">
         <v>3</v>
       </c>
       <c r="K21" t="s">
@@ -2148,7 +2164,7 @@
       <c r="G22" t="s">
         <v>7</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="9">
         <v>1</v>
       </c>
       <c r="K22" t="s">
@@ -2177,7 +2193,7 @@
       <c r="G23" t="s">
         <v>7</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="9">
         <v>1</v>
       </c>
       <c r="K23" t="s">
@@ -2206,11 +2222,40 @@
       <c r="G24" t="s">
         <v>5</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="9">
         <v>2</v>
       </c>
       <c r="K24" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" t="s">
+        <v>154</v>
+      </c>
+      <c r="G25" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="K25" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>